<commit_message>
adding notes, scores, updated stuff for modeling insights
</commit_message>
<xml_diff>
--- a/data/r2_scores.xlsx
+++ b/data/r2_scores.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christopher\OneDrive\Documents\Harvard Grad school\2017-2018 Academic Year\Spring 2018\CSE Capstone Project (APCOMP 297R)\airpred_git\modeling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christopher\OneDrive\Documents\Harvard Grad school\2017-2018 Academic Year\Spring 2018\CSE Capstone Project (APCOMP 297R)\airpred_git\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -408,7 +408,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,7 +469,7 @@
         <v>0.78200000000000003</v>
       </c>
       <c r="C5">
-        <v>0.78200000000000003</v>
+        <v>0.78700000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>